<commit_message>
Updates after code review
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/POCs/APIs_and_db/Dispatcher and Performer/APIs_and_db_Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/POCs/APIs_and_db/New Repos for CR/api-db-dispatcher_v2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3969232D-182A-4AD2-B92E-A6D21CA1B33D}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA9ECB3-DBEC-475C-808D-FF622625D1FB}"/>
   <bookViews>
-    <workbookView xWindow="-24" yWindow="216" windowWidth="23064" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24" yWindow="216" windowWidth="23064" windowHeight="12240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -165,13 +165,13 @@
     <t>APIs_and_db_Dispatcher</t>
   </si>
   <si>
-    <t>https://api.tvmaze.com/search/shows?q=</t>
-  </si>
-  <si>
     <t>The API endpoint to retrieve all shows containing a certain sting in their title</t>
   </si>
   <si>
     <t>Api_Poc</t>
+  </si>
+  <si>
+    <t>TvMazeApiShowsEndpoint</t>
   </si>
 </sst>
 </file>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -620,7 +620,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -643,15 +643,7 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1643,11 +1635,8 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{1F22DC0E-E98D-4833-8A25-930AA98ABFB2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2818,8 +2807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2866,7 +2855,20 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>